<commit_message>
Updated protocol description templates
</commit_message>
<xml_diff>
--- a/data/protocol_descr_australian_template.xlsx
+++ b/data/protocol_descr_australian_template.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20395"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20398"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{605DC2AD-AAF6-427D-BECF-BE080F2AF77A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38A86CCA-0442-43E0-A8EE-78EA60437B15}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="variables" sheetId="1" r:id="rId1"/>
@@ -462,19 +462,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="28.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="28.6640625" customWidth="1"/>
-    <col min="3" max="3" width="29.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="27.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="28.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.7109375" customWidth="1"/>
+    <col min="3" max="3" width="29.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>21</v>
       </c>
@@ -488,7 +488,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>19</v>
       </c>
@@ -496,7 +496,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -504,7 +504,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>13</v>
       </c>
@@ -512,7 +512,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>14</v>
       </c>
@@ -520,7 +520,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -528,7 +528,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -536,7 +536,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>25</v>
       </c>
@@ -557,19 +557,19 @@
       <selection activeCell="A2" sqref="A2:F9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.44140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="78.109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="78.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -589,13 +589,13 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F4" s="5"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F6" s="5"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B9" s="1"/>
     </row>
   </sheetData>
@@ -612,17 +612,17 @@
       <selection activeCell="A2" sqref="A2:XFD13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.44140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="56" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -642,46 +642,46 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F2" s="3"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F3" s="3"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F4" s="3"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F5" s="3"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C6" s="11"/>
       <c r="F6" s="3"/>
     </row>
-    <row r="7" spans="1:7" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
       <c r="F7" s="3"/>
       <c r="G7" s="10"/>
     </row>
-    <row r="8" spans="1:7" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
       <c r="F8" s="3"/>
       <c r="G8" s="10"/>
     </row>
-    <row r="9" spans="1:7" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
       <c r="F9" s="3"/>
       <c r="G9" s="10"/>
     </row>
-    <row r="10" spans="1:7" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
       <c r="F10" s="3"/>
       <c r="G10" s="10"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F11" s="3"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B12" s="1"/>
       <c r="F12" s="3"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B13" s="1"/>
       <c r="F13" s="3"/>
     </row>
@@ -699,15 +699,15 @@
       <selection activeCell="A2" sqref="A2:XFD9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="42" style="9" customWidth="1"/>
-    <col min="3" max="3" width="65.5546875" customWidth="1"/>
+    <col min="3" max="3" width="65.5703125" customWidth="1"/>
     <col min="4" max="4" width="57" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>6</v>
       </c>
@@ -722,83 +722,83 @@
       </c>
       <c r="E1" s="7"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="6"/>
       <c r="B2" s="6"/>
       <c r="C2" s="6"/>
       <c r="D2" s="5"/>
       <c r="E2" s="7"/>
     </row>
-    <row r="3" spans="1:5" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="6"/>
       <c r="B3" s="6"/>
       <c r="C3" s="6"/>
       <c r="D3" s="5"/>
       <c r="E3" s="7"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="6"/>
       <c r="B4" s="6"/>
       <c r="C4" s="5"/>
       <c r="D4" s="5"/>
       <c r="E4" s="7"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="6"/>
       <c r="B5" s="6"/>
       <c r="C5" s="5"/>
       <c r="D5" s="5"/>
       <c r="E5" s="7"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="6"/>
       <c r="B6" s="6"/>
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>
       <c r="E6" s="7"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="5"/>
       <c r="B7" s="5"/>
       <c r="C7" s="5"/>
       <c r="D7" s="5"/>
       <c r="E7" s="7"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="5"/>
       <c r="B8" s="5"/>
       <c r="C8" s="3"/>
       <c r="D8" s="5"/>
       <c r="E8" s="7"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="7"/>
       <c r="B9" s="8"/>
       <c r="D9" s="7"/>
       <c r="E9" s="7"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="7"/>
       <c r="B10" s="8"/>
       <c r="C10" s="7"/>
       <c r="D10" s="7"/>
       <c r="E10" s="7"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="7"/>
       <c r="B11" s="8"/>
       <c r="C11" s="7"/>
       <c r="D11" s="7"/>
       <c r="E11" s="7"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="7"/>
       <c r="B12" s="8"/>
       <c r="C12" s="7"/>
       <c r="D12" s="7"/>
       <c r="E12" s="7"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="7"/>
       <c r="B13" s="8"/>
       <c r="C13" s="7"/>
@@ -813,24 +813,354 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1473B67-BA74-42F8-AEB3-718C16A2BE44}">
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:B67"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A67"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>17</v>
       </c>
       <c r="B1" t="s">
         <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="11">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="11">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="11">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="11">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="11">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="11">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="11">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="11">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="11">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="11">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="11">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="11">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" s="11">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" s="11">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" s="11">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" s="11">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" s="11">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" s="11">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" s="11">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24" s="11">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" s="11">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26" s="11">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A27" s="11">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A28" s="11">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A29" s="11">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A30" s="11">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A31" s="11">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A32" s="11">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" s="11">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34" s="11">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A35" s="11">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A36" s="11">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A37" s="11">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A38" s="11">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A39" s="11">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A40" s="11">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A41" s="11">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A42" s="11">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A43" s="11">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A44" s="11">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A45" s="11">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A46" s="11">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A47" s="11">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A48" s="11">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A49" s="11">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A50" s="11">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A51" s="11">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A52" s="11">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A53" s="11">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A54" s="11">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A55" s="11">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A56" s="11">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A57" s="11">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A58" s="11">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A59" s="11">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A60" s="11">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A61" s="11">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A62" s="11">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A63" s="11">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A64" s="11">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A65" s="11">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A66" s="11">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A67" s="11">
+        <v>66</v>
       </c>
     </row>
   </sheetData>

</xml_diff>